<commit_message>
Added Veenkampen BAM data
Added Veenkampen BAM data
</commit_message>
<xml_diff>
--- a/InstrumentList_v1.1.xlsx
+++ b/InstrumentList_v1.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte035\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\ESG\DOW_MAQ\MAQ_Archive\MAQ-Observations.nl\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400ADCD6-79A6-4BD9-9B4F-2CB5680D5CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C856C9-95E3-4962-9A22-58169927B6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F886D0CD-42D9-4E67-83C9-C1370524BEBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="807">
   <si>
     <t>Stream name</t>
   </si>
@@ -3010,6 +3010,150 @@
   </si>
   <si>
     <t>Added Water Table Depth to Advanced-Soil packages for Veenkampen and Loobos</t>
+  </si>
+  <si>
+    <t>BAM_Conc</t>
+  </si>
+  <si>
+    <t>BAM_Qtot</t>
+  </si>
+  <si>
+    <t>BAM_WS</t>
+  </si>
+  <si>
+    <t>BAM_RH</t>
+  </si>
+  <si>
+    <t>BAM_Delta</t>
+  </si>
+  <si>
+    <t>BAM_AT</t>
+  </si>
+  <si>
+    <t>BAM_E</t>
+  </si>
+  <si>
+    <t>BAM_U</t>
+  </si>
+  <si>
+    <t>BAM_M</t>
+  </si>
+  <si>
+    <t>BAM_I</t>
+  </si>
+  <si>
+    <t>BAM_L</t>
+  </si>
+  <si>
+    <t>BAM_R</t>
+  </si>
+  <si>
+    <t>BAM_N</t>
+  </si>
+  <si>
+    <t>BAM_F</t>
+  </si>
+  <si>
+    <t>BAM_P</t>
+  </si>
+  <si>
+    <t>BAM_D</t>
+  </si>
+  <si>
+    <t>BAM_C</t>
+  </si>
+  <si>
+    <t>BAM_T</t>
+  </si>
+  <si>
+    <r>
+      <t>mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>Added Veenkampen BAM data (18 new streams), added BAM_Conc to Veenkampen Air Quality package</t>
+  </si>
+  <si>
+    <t>Beta Attenuation Mass Monitor 1020</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Total flow volume</t>
+  </si>
+  <si>
+    <t>Wind Speed (BX-591)</t>
+  </si>
+  <si>
+    <t>Relative humidity (BX-593)</t>
+  </si>
+  <si>
+    <t>Air temperature (BX-597)</t>
+  </si>
+  <si>
+    <t>Delta temperature (BX-597)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Telemetry Fault or Interface Fault </t>
+  </si>
+  <si>
+    <t>Flag: External reset or Interface Reset</t>
+  </si>
+  <si>
+    <t>Flag: Maintenance Alarm</t>
+  </si>
+  <si>
+    <t>Flag: Internal Error or Coarse Link Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Power Failure or Processor Reset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Reference Error or Membrane Timeout </t>
+  </si>
+  <si>
+    <t>Flag: Nozzle Error</t>
+  </si>
+  <si>
+    <t>Flag: Flow Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Pressure Drop Alarm or Delta-Pressure Alarm </t>
+  </si>
+  <si>
+    <t>Flag: Deviant Membrane Density Alarm or BAM CAL alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Count Error or Data Error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Tape System Error or Filter Tape Error </t>
   </si>
 </sst>
 </file>
@@ -3455,7 +3599,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603FFA7C-CA32-46E1-B5C1-AB3A403C245A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G194"/>
+  <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7307,6 +7451,366 @@
       </c>
       <c r="G194" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>767</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D195" t="s">
+        <v>642</v>
+      </c>
+      <c r="F195" t="s">
+        <v>733</v>
+      </c>
+      <c r="G195" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>768</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="F196" t="s">
+        <v>728</v>
+      </c>
+      <c r="G196" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>769</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D197" t="s">
+        <v>791</v>
+      </c>
+      <c r="F197" t="s">
+        <v>728</v>
+      </c>
+      <c r="G197" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>770</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="F198" t="s">
+        <v>728</v>
+      </c>
+      <c r="G198" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>771</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="F199" t="s">
+        <v>728</v>
+      </c>
+      <c r="G199" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>772</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="F200" t="s">
+        <v>728</v>
+      </c>
+      <c r="G200" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>773</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D201" t="s">
+        <v>796</v>
+      </c>
+      <c r="F201" t="s">
+        <v>728</v>
+      </c>
+      <c r="G201" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>774</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="F202" t="s">
+        <v>728</v>
+      </c>
+      <c r="G202" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>775</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="F203" t="s">
+        <v>728</v>
+      </c>
+      <c r="G203" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>776</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="F204" t="s">
+        <v>728</v>
+      </c>
+      <c r="G204" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>777</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="F205" t="s">
+        <v>728</v>
+      </c>
+      <c r="G205" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>778</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="F206" t="s">
+        <v>728</v>
+      </c>
+      <c r="G206" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>779</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="F207" t="s">
+        <v>728</v>
+      </c>
+      <c r="G207" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>780</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="F208" t="s">
+        <v>728</v>
+      </c>
+      <c r="G208" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>781</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="F209" t="s">
+        <v>728</v>
+      </c>
+      <c r="G209" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>782</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="F210" t="s">
+        <v>728</v>
+      </c>
+      <c r="G210" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>783</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="F211" t="s">
+        <v>728</v>
+      </c>
+      <c r="G211" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>784</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F212" t="s">
+        <v>728</v>
+      </c>
+      <c r="G212" t="s">
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -16033,7 +16537,7 @@
         <v>755</v>
       </c>
       <c r="B13" s="10">
-        <v>45616</v>
+        <v>45250</v>
       </c>
       <c r="C13" t="s">
         <v>747</v>
@@ -16045,7 +16549,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="10">
-        <v>45627</v>
+        <v>45261</v>
       </c>
       <c r="C14" t="s">
         <v>747</v>
@@ -16057,7 +16561,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="10">
-        <v>45634</v>
+        <v>45268</v>
       </c>
       <c r="C15" t="s">
         <v>747</v>
@@ -16116,6 +16620,15 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
+      <c r="B20" s="10">
+        <v>45638</v>
+      </c>
+      <c r="C20" t="s">
+        <v>747</v>
+      </c>
+      <c r="D20" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Added Veenkampen BAM data (#9)
Added Veenkampen BAM data
</commit_message>
<xml_diff>
--- a/InstrumentList_v1.1.xlsx
+++ b/InstrumentList_v1.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte035\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\ESG\DOW_MAQ\MAQ_Archive\MAQ-Observations.nl\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400ADCD6-79A6-4BD9-9B4F-2CB5680D5CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C856C9-95E3-4962-9A22-58169927B6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F886D0CD-42D9-4E67-83C9-C1370524BEBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="807">
   <si>
     <t>Stream name</t>
   </si>
@@ -3010,6 +3010,150 @@
   </si>
   <si>
     <t>Added Water Table Depth to Advanced-Soil packages for Veenkampen and Loobos</t>
+  </si>
+  <si>
+    <t>BAM_Conc</t>
+  </si>
+  <si>
+    <t>BAM_Qtot</t>
+  </si>
+  <si>
+    <t>BAM_WS</t>
+  </si>
+  <si>
+    <t>BAM_RH</t>
+  </si>
+  <si>
+    <t>BAM_Delta</t>
+  </si>
+  <si>
+    <t>BAM_AT</t>
+  </si>
+  <si>
+    <t>BAM_E</t>
+  </si>
+  <si>
+    <t>BAM_U</t>
+  </si>
+  <si>
+    <t>BAM_M</t>
+  </si>
+  <si>
+    <t>BAM_I</t>
+  </si>
+  <si>
+    <t>BAM_L</t>
+  </si>
+  <si>
+    <t>BAM_R</t>
+  </si>
+  <si>
+    <t>BAM_N</t>
+  </si>
+  <si>
+    <t>BAM_F</t>
+  </si>
+  <si>
+    <t>BAM_P</t>
+  </si>
+  <si>
+    <t>BAM_D</t>
+  </si>
+  <si>
+    <t>BAM_C</t>
+  </si>
+  <si>
+    <t>BAM_T</t>
+  </si>
+  <si>
+    <r>
+      <t>mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>Added Veenkampen BAM data (18 new streams), added BAM_Conc to Veenkampen Air Quality package</t>
+  </si>
+  <si>
+    <t>Beta Attenuation Mass Monitor 1020</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Total flow volume</t>
+  </si>
+  <si>
+    <t>Wind Speed (BX-591)</t>
+  </si>
+  <si>
+    <t>Relative humidity (BX-593)</t>
+  </si>
+  <si>
+    <t>Air temperature (BX-597)</t>
+  </si>
+  <si>
+    <t>Delta temperature (BX-597)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Telemetry Fault or Interface Fault </t>
+  </si>
+  <si>
+    <t>Flag: External reset or Interface Reset</t>
+  </si>
+  <si>
+    <t>Flag: Maintenance Alarm</t>
+  </si>
+  <si>
+    <t>Flag: Internal Error or Coarse Link Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Power Failure or Processor Reset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Reference Error or Membrane Timeout </t>
+  </si>
+  <si>
+    <t>Flag: Nozzle Error</t>
+  </si>
+  <si>
+    <t>Flag: Flow Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Pressure Drop Alarm or Delta-Pressure Alarm </t>
+  </si>
+  <si>
+    <t>Flag: Deviant Membrane Density Alarm or BAM CAL alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Count Error or Data Error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag: Tape System Error or Filter Tape Error </t>
   </si>
 </sst>
 </file>
@@ -3455,7 +3599,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603FFA7C-CA32-46E1-B5C1-AB3A403C245A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G194"/>
+  <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7307,6 +7451,366 @@
       </c>
       <c r="G194" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>767</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D195" t="s">
+        <v>642</v>
+      </c>
+      <c r="F195" t="s">
+        <v>733</v>
+      </c>
+      <c r="G195" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>768</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="F196" t="s">
+        <v>728</v>
+      </c>
+      <c r="G196" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>769</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D197" t="s">
+        <v>791</v>
+      </c>
+      <c r="F197" t="s">
+        <v>728</v>
+      </c>
+      <c r="G197" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>770</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="F198" t="s">
+        <v>728</v>
+      </c>
+      <c r="G198" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>771</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="F199" t="s">
+        <v>728</v>
+      </c>
+      <c r="G199" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>772</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="F200" t="s">
+        <v>728</v>
+      </c>
+      <c r="G200" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>773</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D201" t="s">
+        <v>796</v>
+      </c>
+      <c r="F201" t="s">
+        <v>728</v>
+      </c>
+      <c r="G201" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>774</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="F202" t="s">
+        <v>728</v>
+      </c>
+      <c r="G202" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>775</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="F203" t="s">
+        <v>728</v>
+      </c>
+      <c r="G203" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>776</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="F204" t="s">
+        <v>728</v>
+      </c>
+      <c r="G204" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>777</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="F205" t="s">
+        <v>728</v>
+      </c>
+      <c r="G205" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>778</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="F206" t="s">
+        <v>728</v>
+      </c>
+      <c r="G206" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>779</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="F207" t="s">
+        <v>728</v>
+      </c>
+      <c r="G207" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>780</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="F208" t="s">
+        <v>728</v>
+      </c>
+      <c r="G208" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>781</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="F209" t="s">
+        <v>728</v>
+      </c>
+      <c r="G209" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>782</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="F210" t="s">
+        <v>728</v>
+      </c>
+      <c r="G210" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>783</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="F211" t="s">
+        <v>728</v>
+      </c>
+      <c r="G211" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>784</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F212" t="s">
+        <v>728</v>
+      </c>
+      <c r="G212" t="s">
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -16033,7 +16537,7 @@
         <v>755</v>
       </c>
       <c r="B13" s="10">
-        <v>45616</v>
+        <v>45250</v>
       </c>
       <c r="C13" t="s">
         <v>747</v>
@@ -16045,7 +16549,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="10">
-        <v>45627</v>
+        <v>45261</v>
       </c>
       <c r="C14" t="s">
         <v>747</v>
@@ -16057,7 +16561,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="10">
-        <v>45634</v>
+        <v>45268</v>
       </c>
       <c r="C15" t="s">
         <v>747</v>
@@ -16116,6 +16620,15 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
+      <c r="B20" s="10">
+        <v>45638</v>
+      </c>
+      <c r="C20" t="s">
+        <v>747</v>
+      </c>
+      <c r="D20" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Updated metadata with distance sensor
</commit_message>
<xml_diff>
--- a/InstrumentList_v1.1.xlsx
+++ b/InstrumentList_v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\ESG\DOW_MAQ\MAQ_Archive\MAQ-Observations.nl\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCAEB14-F99A-4DBD-B9FE-02508F759E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495FC12D-AD84-46FA-8F1B-D4CFE893802B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{F886D0CD-42D9-4E67-83C9-C1370524BEBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4777" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4785" uniqueCount="1015">
   <si>
     <t>Stream name</t>
   </si>
@@ -3766,6 +3766,18 @@
   </si>
   <si>
     <t>Amsterdam: Included all 23 stations of Distributed Network. Added Distributed Network as ADVANCED download package. Added Veenkampen and Amsterdam to ADVANCED Leaf Wetness package</t>
+  </si>
+  <si>
+    <t>DH_1_1_1</t>
+  </si>
+  <si>
+    <t>Distance sensor</t>
+  </si>
+  <si>
+    <t>Distance / Grass height</t>
+  </si>
+  <si>
+    <t>Added distance sensor Veenkampen</t>
   </si>
 </sst>
 </file>
@@ -4214,9 +4226,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603FFA7C-CA32-46E1-B5C1-AB3A403C245A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G215"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8540,6 +8554,26 @@
         <v>728</v>
       </c>
       <c r="G214" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F215" t="s">
+        <v>724</v>
+      </c>
+      <c r="G215" t="s">
         <v>846</v>
       </c>
     </row>
@@ -19942,7 +19976,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C5BFE-6C5D-49EF-B6DC-8FDF9610AF86}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20325,6 +20359,17 @@
         <v>1010</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="10">
+        <v>45859</v>
+      </c>
+      <c r="C41" t="s">
+        <v>740</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1014</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{4C6C8172-E3B1-4460-AE30-8C1A4FB4F619}"/>

</xml_diff>